<commit_message>
Merge start: 1st Row1, other Row2
Merge start from:  1st file Row1, other  file Row2
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -15,7 +15,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>kind</t>
+  </si>
+  <si>
+    <t>num</t>
+  </si>
   <si>
     <t>Apples</t>
   </si>
@@ -380,7 +389,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -389,222 +398,234 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="n">
-        <v>42099.56530092593</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="n">
         <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="n">
-        <v>42099.15373842593</v>
+        <v>42099.56530092593</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="n">
         <v>1</v>
-      </c>
-      <c r="C2" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="n">
-        <v>42100.53253472222</v>
+        <v>42099.15373842593</v>
       </c>
       <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="n">
         <v>2</v>
-      </c>
-      <c r="C3" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="n">
-        <v>42102.37480324074</v>
+        <v>42100.53253472222</v>
       </c>
       <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="n">
         <v>3</v>
       </c>
-      <c r="C4" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="n">
-        <v>42104.08819444444</v>
-      </c>
-      <c r="B5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" t="n">
-        <v>5</v>
-      </c>
-    </row>
+    </row>
+    <row r="5" spans="1:3"/>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="n">
-        <v>42104.75737268518</v>
+        <v>42102.37480324074</v>
       </c>
       <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="n">
         <v>4</v>
-      </c>
-      <c r="C6" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1" t="n">
-        <v>42104.11164351852</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="n">
-        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="n">
-        <v>0</v>
+        <v>42104.08819444444</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C8" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="n">
-        <v>2</v>
+        <v>42104.75737268518</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="n">
-        <v>3</v>
+        <v>42104.11164351852</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1" t="n">
-        <v>42104.08819444444</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C11" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="n">
-        <v>42104.75737268518</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C12" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="n">
-        <v>42104.11164351852</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C13" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1" t="n">
-        <v>2</v>
+        <v>42104.08819444444</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C15" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="n">
-        <v>42104.08819444444</v>
+        <v>42104.75737268518</v>
       </c>
       <c r="B16" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C16" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="n">
-        <v>42104.75737268518</v>
+        <v>42104.11164351852</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C17" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="n">
-        <v>42104.11164351852</v>
+        <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C18" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1" t="n">
+        <v>42104.08819444444</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="n">
+        <v>42104.75737268518</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1" t="n">
+        <v>42104.11164351852</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" t="n">
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="n">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="1" t="n">
+    <row r="25" spans="1:3">
+      <c r="A25" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" t="n">
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="n">
         <v>20</v>
       </c>
     </row>

</xml_diff>